<commit_message>
update read me file
</commit_message>
<xml_diff>
--- a/Documents/PHPTravel_TestCase.xlsx
+++ b/Documents/PHPTravel_TestCase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laitpham\Desktop\APlus-BabySharks1\APlus-BabySharks1\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laitpham\Desktop\Internship_BDD_Cucumber_Framework\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846C3AD9-7331-4BCC-B52C-7AAA5EC1E5D6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1983616-C7FB-489D-9310-B210E5E5A3A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{A9500B81-C06F-483B-A7AE-E2172403D26B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{A9500B81-C06F-483B-A7AE-E2172403D26B}"/>
   </bookViews>
   <sheets>
     <sheet name="Front End" sheetId="1" r:id="rId1"/>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="172">
   <si>
     <t>Area</t>
   </si>
@@ -980,51 +980,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1035,29 +990,74 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1375,7 +1375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC6FDA77-4191-4938-A722-4B8307AF83E2}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -1418,16 +1418,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="7"/>
@@ -1442,10 +1442,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7">
         <v>2</v>
@@ -1458,10 +1458,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7">
         <v>3</v>
@@ -1474,10 +1474,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7">
         <v>4</v>
@@ -1490,19 +1490,19 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="24" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="7">
@@ -1516,11 +1516,11 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="7">
         <v>2</v>
       </c>
@@ -1532,11 +1532,11 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="7">
         <v>3</v>
       </c>
@@ -1548,11 +1548,11 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
       <c r="F9" s="9">
         <v>4</v>
       </c>
@@ -1564,16 +1564,16 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="26" t="s">
         <v>32</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -1590,10 +1590,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="21"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="26"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7">
         <v>2</v>
@@ -1606,10 +1606,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="21"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7">
         <v>3</v>
@@ -1622,19 +1622,19 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="26" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="26" t="s">
         <v>20</v>
       </c>
       <c r="F13" s="7">
@@ -1648,11 +1648,11 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="21"/>
+      <c r="E14" s="26"/>
       <c r="F14" s="7">
         <v>2</v>
       </c>
@@ -1664,11 +1664,11 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="21"/>
+      <c r="E15" s="26"/>
       <c r="F15" s="7">
         <v>3</v>
       </c>
@@ -1680,17 +1680,17 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="26" t="s">
         <v>47</v>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="26" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="7">
@@ -1704,11 +1704,11 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="21"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="7">
         <v>2</v>
       </c>
@@ -1720,11 +1720,11 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="21"/>
+      <c r="E18" s="26"/>
       <c r="F18" s="7">
         <v>3</v>
       </c>
@@ -1736,7 +1736,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="27" t="s">
         <v>57</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -1746,7 +1746,7 @@
         <v>59</v>
       </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="26" t="s">
         <v>20</v>
       </c>
       <c r="F19" s="7">
@@ -1760,11 +1760,11 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="31"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="21"/>
+      <c r="E20" s="26"/>
       <c r="F20" s="7">
         <v>2</v>
       </c>
@@ -1776,11 +1776,11 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="31"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="21"/>
+      <c r="E21" s="26"/>
       <c r="F21" s="7">
         <v>3</v>
       </c>
@@ -1792,11 +1792,11 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="21"/>
+      <c r="E22" s="26"/>
       <c r="F22" s="7">
         <v>4</v>
       </c>
@@ -1808,11 +1808,11 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="21"/>
+      <c r="E23" s="26"/>
       <c r="F23" s="7">
         <v>5</v>
       </c>
@@ -1824,17 +1824,17 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="26" t="s">
         <v>70</v>
       </c>
       <c r="D24" s="7"/>
-      <c r="E24" s="21" t="s">
+      <c r="E24" s="26" t="s">
         <v>20</v>
       </c>
       <c r="F24" s="7">
@@ -1848,11 +1848,11 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="21"/>
+      <c r="E25" s="26"/>
       <c r="F25" s="7">
         <v>2</v>
       </c>
@@ -1862,11 +1862,11 @@
       <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
       <c r="D26" s="7"/>
-      <c r="E26" s="21"/>
+      <c r="E26" s="26"/>
       <c r="F26" s="7">
         <v>3</v>
       </c>
@@ -1878,11 +1878,11 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="21"/>
+      <c r="E27" s="26"/>
       <c r="F27" s="7">
         <v>4</v>
       </c>
@@ -1894,11 +1894,11 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
       <c r="D28" s="7"/>
-      <c r="E28" s="21"/>
+      <c r="E28" s="26"/>
       <c r="F28" s="7">
         <v>5</v>
       </c>
@@ -1910,153 +1910,153 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="33"/>
-      <c r="E29" s="32" t="s">
+      <c r="D29" s="18"/>
+      <c r="E29" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="18">
         <v>1</v>
       </c>
-      <c r="G29" s="34" t="s">
+      <c r="G29" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="H29" s="34" t="s">
+      <c r="H29" s="19" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="33">
+      <c r="A30" s="31"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="18">
         <v>2</v>
       </c>
-      <c r="G30" s="35" t="s">
+      <c r="G30" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="H30" s="33"/>
+      <c r="H30" s="18"/>
     </row>
     <row r="31" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="33">
+      <c r="A31" s="31"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="18">
         <v>3</v>
       </c>
-      <c r="G31" s="35" t="s">
+      <c r="G31" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="H31" s="35" t="s">
+      <c r="H31" s="20" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="33">
+      <c r="A32" s="31"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="18">
         <v>4</v>
       </c>
-      <c r="G32" s="36" t="s">
+      <c r="G32" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="H32" s="35" t="s">
+      <c r="H32" s="20" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="32" t="s">
+      <c r="A33" s="31"/>
+      <c r="B33" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="32" t="s">
+      <c r="C33" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="33"/>
-      <c r="E33" s="32" t="s">
+      <c r="D33" s="18"/>
+      <c r="E33" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="33">
+      <c r="F33" s="18">
         <v>1</v>
       </c>
-      <c r="G33" s="34" t="s">
+      <c r="G33" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="H33" s="34" t="s">
+      <c r="H33" s="19" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="19"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="33">
+      <c r="A34" s="31"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="18">
         <v>2</v>
       </c>
-      <c r="G34" s="35" t="s">
+      <c r="G34" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="H34" s="33"/>
+      <c r="H34" s="18"/>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="33">
+      <c r="A35" s="31"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="18">
         <v>3</v>
       </c>
-      <c r="G35" s="35" t="s">
+      <c r="G35" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="H35" s="33"/>
+      <c r="H35" s="18"/>
     </row>
     <row r="36" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="33">
+      <c r="A36" s="32"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="18">
         <v>4</v>
       </c>
-      <c r="G36" s="35" t="s">
+      <c r="G36" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="H36" s="36" t="s">
+      <c r="H36" s="21" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="26" t="s">
         <v>95</v>
       </c>
       <c r="D37" s="7"/>
-      <c r="E37" s="21" t="s">
+      <c r="E37" s="26" t="s">
         <v>20</v>
       </c>
       <c r="F37" s="7">
@@ -2070,11 +2070,11 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A38" s="19"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
       <c r="D38" s="7"/>
-      <c r="E38" s="21"/>
+      <c r="E38" s="26"/>
       <c r="F38" s="7">
         <v>2</v>
       </c>
@@ -2084,11 +2084,11 @@
       <c r="H38" s="7"/>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="19"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
+      <c r="A39" s="31"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
       <c r="D39" s="7"/>
-      <c r="E39" s="21"/>
+      <c r="E39" s="26"/>
       <c r="F39" s="7">
         <v>3</v>
       </c>
@@ -2100,11 +2100,11 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
+      <c r="A40" s="32"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="21"/>
+      <c r="E40" s="26"/>
       <c r="F40" s="7">
         <v>4</v>
       </c>
@@ -2117,19 +2117,17 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="E33:E36"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="C37:C40"/>
     <mergeCell ref="E19:E23"/>
     <mergeCell ref="E24:E28"/>
     <mergeCell ref="E29:E32"/>
@@ -2144,17 +2142,19 @@
     <mergeCell ref="A19:A23"/>
     <mergeCell ref="A24:A28"/>
     <mergeCell ref="A29:A36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="E33:E36"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="E37:E40"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2165,7 +2165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCBEA60-37DA-4B83-B7FE-2EB8C201602A}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A36" sqref="A36:G40"/>
     </sheetView>
   </sheetViews>
@@ -2202,10 +2202,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="31">
+      <c r="A2" s="33">
         <v>1</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="33" t="s">
         <v>109</v>
       </c>
       <c r="C2" s="14"/>
@@ -2220,8 +2220,8 @@
       <c r="H2" s="16"/>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="14"/>
       <c r="D3" s="14">
         <v>2</v>
@@ -2234,8 +2234,8 @@
       <c r="H3" s="16"/>
     </row>
     <row r="4" spans="1:8" ht="240" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="14"/>
       <c r="D4" s="14">
         <v>3</v>
@@ -2250,10 +2250,10 @@
       <c r="H4" s="16"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="31">
+      <c r="A5" s="33">
         <v>2</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="33" t="s">
         <v>114</v>
       </c>
       <c r="C5" s="14"/>
@@ -2268,8 +2268,8 @@
       <c r="H5" s="16"/>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14">
         <v>2</v>
@@ -2284,8 +2284,8 @@
       <c r="H6" s="16"/>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14">
         <v>3</v>
@@ -2300,8 +2300,8 @@
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14">
         <v>4</v>
@@ -2316,13 +2316,13 @@
       <c r="H8" s="16"/>
     </row>
     <row r="9" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
+      <c r="A9" s="33">
         <v>3</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="25" t="s">
         <v>171</v>
       </c>
       <c r="D9" s="14">
@@ -2336,9 +2336,9 @@
       <c r="H9" s="16"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="26"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="14">
         <v>2</v>
       </c>
@@ -2352,9 +2352,9 @@
       <c r="H10" s="16"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="26"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="14">
         <v>3</v>
       </c>
@@ -2368,9 +2368,9 @@
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="26"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="14">
         <v>4</v>
       </c>
@@ -2384,9 +2384,9 @@
       <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="26"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="14">
         <v>5</v>
       </c>
@@ -2400,9 +2400,9 @@
       <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="26"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="14">
         <v>6</v>
       </c>
@@ -2416,9 +2416,9 @@
       <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="27"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="38"/>
       <c r="D15" s="14">
         <v>7</v>
       </c>
@@ -2432,13 +2432,13 @@
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="31">
+      <c r="A16" s="33">
         <v>4</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="33" t="s">
         <v>135</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="25" t="s">
         <v>171</v>
       </c>
       <c r="D16" s="14">
@@ -2452,9 +2452,9 @@
       <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="14">
         <v>2</v>
       </c>
@@ -2468,9 +2468,9 @@
       <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="14">
         <v>3</v>
       </c>
@@ -2482,9 +2482,9 @@
       <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="26"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="14">
         <v>4</v>
       </c>
@@ -2496,9 +2496,9 @@
       <c r="H19" s="16"/>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="27"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="14">
         <v>5</v>
       </c>
@@ -2512,13 +2512,13 @@
       <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="28">
+      <c r="A21" s="34">
         <v>5</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="25" t="s">
         <v>171</v>
       </c>
       <c r="D21" s="14">
@@ -2532,9 +2532,9 @@
       <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="26"/>
+      <c r="A22" s="35"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="14">
         <v>2</v>
       </c>
@@ -2548,9 +2548,9 @@
       <c r="H22" s="16"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="26"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="14">
         <v>3</v>
       </c>
@@ -2562,9 +2562,9 @@
       <c r="H23" s="16"/>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="26"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="37"/>
       <c r="D24" s="14">
         <v>4</v>
       </c>
@@ -2576,9 +2576,9 @@
       <c r="H24" s="16"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="27"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="38"/>
       <c r="D25" s="14">
         <v>5</v>
       </c>
@@ -2592,13 +2592,13 @@
       <c r="H25" s="16"/>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="28">
+      <c r="A26" s="34">
         <v>6</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="25" t="s">
         <v>171</v>
       </c>
       <c r="D26" s="14">
@@ -2612,9 +2612,9 @@
       <c r="H26" s="16"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="26"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="37"/>
       <c r="D27" s="14">
         <v>2</v>
       </c>
@@ -2628,9 +2628,9 @@
       <c r="H27" s="16"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="26"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="14">
         <v>3</v>
       </c>
@@ -2642,9 +2642,9 @@
       <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="26"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="14">
         <v>4</v>
       </c>
@@ -2656,9 +2656,9 @@
       <c r="H29" s="16"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="27"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="38"/>
       <c r="D30" s="14">
         <v>5</v>
       </c>
@@ -2672,13 +2672,13 @@
       <c r="H30" s="16"/>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="28">
+      <c r="A31" s="34">
         <v>7</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="25" t="s">
         <v>171</v>
       </c>
       <c r="D31" s="14">
@@ -2692,9 +2692,9 @@
       <c r="H31" s="16"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="26"/>
+      <c r="A32" s="35"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="37"/>
       <c r="D32" s="14">
         <v>2</v>
       </c>
@@ -2706,9 +2706,9 @@
       <c r="H32" s="16"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="26"/>
+      <c r="A33" s="35"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="14">
         <v>3</v>
       </c>
@@ -2720,9 +2720,9 @@
       <c r="H33" s="16"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="26"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="37"/>
       <c r="D34" s="14">
         <v>4</v>
       </c>
@@ -2734,9 +2734,9 @@
       <c r="H34" s="16"/>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="27"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="38"/>
       <c r="D35" s="14">
         <v>5</v>
       </c>
@@ -2750,91 +2750,91 @@
       <c r="H35" s="16"/>
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="37">
+      <c r="A36" s="42">
         <v>8</v>
       </c>
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="C36" s="38" t="s">
+      <c r="C36" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="D36" s="39">
+      <c r="D36" s="22">
         <v>1</v>
       </c>
-      <c r="E36" s="40" t="s">
+      <c r="E36" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
       <c r="H36" s="16"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="39">
+      <c r="A37" s="43"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="22">
         <v>2</v>
       </c>
-      <c r="E37" s="40" t="s">
+      <c r="E37" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
       <c r="H37" s="16"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="39">
+      <c r="A38" s="43"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="22">
         <v>3</v>
       </c>
-      <c r="E38" s="40" t="s">
+      <c r="E38" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
       <c r="H38" s="16"/>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="39">
+      <c r="A39" s="43"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="22">
         <v>4</v>
       </c>
-      <c r="E39" s="40" t="s">
+      <c r="E39" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
       <c r="H39" s="16"/>
     </row>
     <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="43"/>
-      <c r="B40" s="43"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="39">
+      <c r="A40" s="44"/>
+      <c r="B40" s="44"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="22">
         <v>5</v>
       </c>
-      <c r="E40" s="40" t="s">
+      <c r="E40" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="F40" s="40" t="s">
+      <c r="F40" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="G40" s="40"/>
+      <c r="G40" s="23"/>
       <c r="H40" s="16"/>
     </row>
     <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="28">
+      <c r="A41" s="34">
         <v>9</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="C41" s="23" t="s">
+      <c r="C41" s="25" t="s">
         <v>171</v>
       </c>
       <c r="D41" s="14">
@@ -2848,9 +2848,9 @@
       <c r="H41" s="16"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="26"/>
+      <c r="A42" s="35"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="37"/>
       <c r="D42" s="14">
         <v>2</v>
       </c>
@@ -2862,9 +2862,9 @@
       <c r="H42" s="16"/>
     </row>
     <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="26"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="37"/>
       <c r="D43" s="14">
         <v>3</v>
       </c>
@@ -2878,9 +2878,9 @@
       <c r="H43" s="16"/>
     </row>
     <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="26"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="37"/>
       <c r="D44" s="14">
         <v>4</v>
       </c>
@@ -2894,9 +2894,9 @@
       <c r="H44" s="16"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="27"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="38"/>
       <c r="D45" s="14">
         <v>5</v>
       </c>
@@ -2910,13 +2910,13 @@
       <c r="H45" s="16"/>
     </row>
     <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="28">
+      <c r="A46" s="34">
         <v>10</v>
       </c>
-      <c r="B46" s="28" t="s">
+      <c r="B46" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="C46" s="23" t="s">
+      <c r="C46" s="25" t="s">
         <v>171</v>
       </c>
       <c r="D46" s="14">
@@ -2930,9 +2930,9 @@
       <c r="H46" s="16"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="29"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="26"/>
+      <c r="A47" s="35"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="37"/>
       <c r="D47" s="14">
         <v>2</v>
       </c>
@@ -2944,9 +2944,9 @@
       <c r="H47" s="16"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="29"/>
-      <c r="B48" s="29"/>
-      <c r="C48" s="26"/>
+      <c r="A48" s="35"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="37"/>
       <c r="D48" s="14">
         <v>3</v>
       </c>
@@ -2960,9 +2960,9 @@
       <c r="H48" s="16"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
-      <c r="B49" s="29"/>
-      <c r="C49" s="26"/>
+      <c r="A49" s="35"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="37"/>
       <c r="D49" s="14">
         <v>4</v>
       </c>
@@ -2976,9 +2976,9 @@
       <c r="H49" s="16"/>
     </row>
     <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="29"/>
-      <c r="B50" s="29"/>
-      <c r="C50" s="26"/>
+      <c r="A50" s="35"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="37"/>
       <c r="D50" s="14">
         <v>5</v>
       </c>
@@ -2992,9 +2992,9 @@
       <c r="H50" s="16"/>
     </row>
     <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
-      <c r="B51" s="30"/>
-      <c r="C51" s="27"/>
+      <c r="A51" s="36"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="38"/>
       <c r="D51" s="14">
         <v>6</v>
       </c>
@@ -3009,18 +3009,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
     <mergeCell ref="C46:C51"/>
     <mergeCell ref="A46:A51"/>
     <mergeCell ref="B46:B51"/>
@@ -3037,6 +3025,18 @@
     <mergeCell ref="B36:B40"/>
     <mergeCell ref="A41:A45"/>
     <mergeCell ref="B41:B45"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="B9:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>